<commit_message>
added draft cap statements
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-CDEX\input\resources-spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8983270-486E-4372-8728-81A35E3A705F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40311E3-221F-47E7-AE7B-FDD912C85524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="540" windowWidth="37935" windowHeight="15795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37590" yWindow="1620" windowWidth="37935" windowHeight="15795" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -482,13 +480,13 @@
   </si>
   <si>
     <t>The  Da Vinci CDex Data Consumer  **SHALL**:
-1. Support at least on of the two FHIR transaction approaches for requesting information as defined in this Guide:
+1. Support at least one of the two FHIR transaction approaches for requesting information as defined in this Guide:
      1. Direct Query
      1. Task Based Approachs
-1. Support json source formats for all Da Vinci Notification interactions.
+1. Support json source formats for all Da Vinci CDex interactions.
 1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
 The  Da Vinci CDex Data Consumer  **SHOULD**:
-1. Support xml source formats for all Da Vinci Notification interactions.</t>
+1. Support xml source formats for all Da Vinci CDex interactions.</t>
   </si>
 </sst>
 </file>
@@ -1610,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1702,7 +1700,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1753,7 +1751,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1850,7 +1848,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2059,7 +2057,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D29" sqref="D29"/>
+      <selection pane="topRight" sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2281,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418CE29-40DC-476E-89CD-A42CEC26847E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U18" sqref="U18:V18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated menu, edit to background, spec and add scenario
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-CDEX\input\resources-spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40311E3-221F-47E7-AE7B-FDD912C85524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E2A0CB-D3B5-9540-B330-E32BF4A6FC5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37590" yWindow="1620" windowWidth="37935" windowHeight="15795" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>Element</t>
   </si>
@@ -410,9 +410,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide-hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
   </si>
   <si>
     <t>HRex Task Data Request Profile</t>
@@ -488,12 +485,21 @@
 The  Da Vinci CDex Data Consumer  **SHOULD**:
 1. Support xml source formats for all Da Vinci CDex interactions.</t>
   </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/StructureDefinition/cdex-task-data-request</t>
+  </si>
+  <si>
+    <t>CDex Task Data Request Profile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +570,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -610,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -638,6 +651,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -959,9 +973,9 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -969,24 +983,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -994,7 +1008,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
@@ -1002,7 +1016,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -1010,7 +1024,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>93</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>95</v>
       </c>
@@ -1026,14 +1040,14 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="C13" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1052,21 +1066,21 @@
       <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1098,56 +1112,56 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="D9"/>
       <c r="E9"/>
@@ -1155,7 +1169,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -1164,7 +1178,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="D11"/>
       <c r="E11"/>
@@ -1172,14 +1186,14 @@
       <c r="H11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="D13"/>
       <c r="E13"/>
@@ -1187,27 +1201,27 @@
       <c r="H13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="D17"/>
       <c r="E17"/>
@@ -1215,14 +1229,14 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="D19"/>
       <c r="E19"/>
@@ -1231,7 +1245,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="D20"/>
       <c r="E20"/>
@@ -1239,20 +1253,20 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="H22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -1260,7 +1274,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
@@ -1268,7 +1282,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
@@ -1276,25 +1290,25 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="D29"/>
       <c r="E29"/>
@@ -1303,7 +1317,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="D30"/>
       <c r="E30"/>
@@ -1312,7 +1326,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="D31"/>
       <c r="E31"/>
@@ -1321,7 +1335,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="D32"/>
       <c r="E32"/>
@@ -1330,203 +1344,203 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="3:10" s="1" customFormat="1">
+    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="3:10">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="3:10" s="1" customFormat="1">
+    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="3:10" s="1" customFormat="1">
+    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="3:10" s="1" customFormat="1">
+    <row r="40" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H41" s="5"/>
       <c r="I41" s="9"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H42" s="5"/>
       <c r="I42" s="9"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="43" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H43" s="5"/>
       <c r="I43" s="9"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="3:10" s="1" customFormat="1">
+    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="3:10" s="1" customFormat="1">
+    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C45" s="11"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="3:10" s="1" customFormat="1">
+    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C46" s="11"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="3:10" s="1" customFormat="1">
+    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C47" s="11"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="3:10" s="1" customFormat="1">
+    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C48" s="11"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="3:10" s="1" customFormat="1">
+    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C49" s="11"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="3:10" s="1" customFormat="1">
+    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="3:10" s="1" customFormat="1">
+    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="3:10" s="1" customFormat="1">
+    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="3:10" s="1" customFormat="1">
+    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="3:10" s="1" customFormat="1">
+    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="3:10" s="1" customFormat="1">
+    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="3:10" s="1" customFormat="1">
+    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="3:10" s="1" customFormat="1">
+    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="3:10" s="1" customFormat="1">
+    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="3:10" s="1" customFormat="1">
+    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="3:10" s="1" customFormat="1">
+    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="3:10" s="1" customFormat="1">
+    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="3:10" s="1" customFormat="1">
+    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C62" s="11"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="3:10" s="1" customFormat="1">
+    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C63" s="11"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="3:10" s="1" customFormat="1">
+    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="3:16" s="1" customFormat="1">
+    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C65" s="11"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="3:16" s="1" customFormat="1">
+    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C66" s="11"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="3:16" s="1" customFormat="1">
+    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C67" s="11"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="3:16" s="1" customFormat="1">
+    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C68" s="11"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="3:16" s="1" customFormat="1">
+    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="3:16" ht="15.75">
+    <row r="70" spans="3:16" ht="16" x14ac:dyDescent="0.2">
       <c r="C70" s="10"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -1538,62 +1552,62 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="3:16" s="1" customFormat="1">
+    <row r="71" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="3:16" s="1" customFormat="1">
+    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="3:16" s="1" customFormat="1">
+    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="3:16" s="1" customFormat="1">
+    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="3:16" s="1" customFormat="1">
+    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="3:16" s="1" customFormat="1">
+    <row r="76" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="3:16" s="1" customFormat="1">
+    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="3:16" s="1" customFormat="1">
+    <row r="78" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="3:16" s="1" customFormat="1" ht="15.75">
+    <row r="79" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H79" s="5"/>
       <c r="I79" s="9"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="3:16" s="1" customFormat="1">
+    <row r="80" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="8:10" s="1" customFormat="1">
+    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="8:10" s="1" customFormat="1">
+    <row r="82" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
@@ -1612,13 +1626,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +1648,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -1642,7 +1656,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1650,7 +1664,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" customHeight="1">
+    <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1658,7 +1672,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1680,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1674,15 +1688,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="207.75" customHeight="1">
+    <row r="8" spans="1:2" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="103.5" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1703,12 +1717,12 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1719,7 +1733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -1730,7 +1744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -1750,19 +1764,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1776,27 +1790,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="30">
-      <c r="A3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -1806,32 +1820,45 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -1851,23 +1878,23 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="14" width="17.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="1" customWidth="1"/>
-    <col min="16" max="19" width="17.42578125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="20.42578125" style="1" customWidth="1"/>
-    <col min="22" max="25" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="17.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="1" customWidth="1"/>
+    <col min="16" max="19" width="17.5" style="1" customWidth="1"/>
+    <col min="20" max="21" width="20.5" style="1" customWidth="1"/>
+    <col min="22" max="25" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" thickBot="1">
+    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1944,7 +1971,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="45.75" thickTop="1">
+    <row r="2" spans="1:25" ht="33" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
@@ -1952,21 +1979,21 @@
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="30">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -1974,26 +2001,26 @@
         <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="22:25" ht="18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="22:25" ht="18" x14ac:dyDescent="0.2">
       <c r="V24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
     </row>
-    <row r="27" spans="22:25" ht="18">
+    <row r="27" spans="22:25" ht="18" x14ac:dyDescent="0.2">
       <c r="Y27" s="7"/>
     </row>
   </sheetData>
@@ -2010,16 +2037,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2036,13 +2063,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -2060,16 +2087,16 @@
       <selection pane="topRight" sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2086,19 +2113,19 @@
         <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2117,7 +2144,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2136,7 +2163,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2155,7 +2182,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2174,7 +2201,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2193,7 +2220,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2212,7 +2239,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2231,7 +2258,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2250,7 +2277,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2279,17 +2306,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418CE29-40DC-476E-89CD-A42CEC26847E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2301,9 +2328,9 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -2311,25 +2338,25 @@
       <c r="C2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>26</v>
@@ -2351,34 +2378,34 @@
       <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -2464,29 +2491,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="12"/>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA4" s="12"/>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z5" s="5"/>
       <c r="AA5" s="12"/>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="12"/>
     </row>
-    <row r="7" spans="1:28" ht="18.95" customHeight="1">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7" s="6"/>
       <c r="E7"/>
@@ -2496,7 +2523,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="12"/>
     </row>
-    <row r="8" spans="1:28" ht="18.95" customHeight="1">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="C8"/>
       <c r="E8"/>
@@ -2505,7 +2532,7 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="18.95" customHeight="1">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9"/>
       <c r="E9"/>
@@ -2516,7 +2543,7 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="18.95" customHeight="1">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -2532,7 +2559,7 @@
       <c r="AA10" s="12"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="18.95" customHeight="1">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="C11"/>
       <c r="E11"/>
@@ -2544,7 +2571,7 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="18.95" customHeight="1">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12"/>
       <c r="C12"/>
       <c r="E12"/>
@@ -2552,7 +2579,7 @@
       <c r="AA12" s="12"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="18.95" customHeight="1">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -2562,7 +2589,7 @@
       <c r="AA13" s="12"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="18.95" customHeight="1">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -2572,12 +2599,12 @@
       <c r="Z14" s="5"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="12"/>
     </row>
-    <row r="16" spans="1:28" ht="18.95" customHeight="1">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="C16"/>
       <c r="E16"/>
@@ -2585,7 +2612,7 @@
       <c r="AA16" s="12"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="2:28" ht="18.95" customHeight="1">
+    <row r="17" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -2596,7 +2623,7 @@
       <c r="AA17" s="12"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="2:28" ht="18.95" customHeight="1">
+    <row r="18" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
@@ -2607,7 +2634,7 @@
       <c r="AA18" s="12"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="2:28" ht="18.95" customHeight="1">
+    <row r="19" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="C19"/>
       <c r="J19"/>
@@ -2617,7 +2644,7 @@
       <c r="AA19" s="12"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="2:28" ht="18.95" customHeight="1">
+    <row r="20" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
       <c r="X20"/>
@@ -2626,7 +2653,7 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="2:28" ht="18.95" customHeight="1">
+    <row r="21" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -2635,21 +2662,21 @@
       <c r="Z21" s="5"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="2:28" ht="18.95" customHeight="1">
+    <row r="22" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22"/>
       <c r="C22"/>
       <c r="E22"/>
       <c r="Z22"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="2:28" ht="18.95" customHeight="1">
+    <row r="23" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23"/>
       <c r="E23"/>
       <c r="J23" s="6"/>
       <c r="Y23"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="2:28" ht="18.95" customHeight="1">
+    <row r="24" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24"/>
       <c r="C24"/>
       <c r="E24"/>
@@ -2658,7 +2685,7 @@
       <c r="AA24" s="12"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="2:28" ht="18.95" customHeight="1">
+    <row r="25" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25"/>
       <c r="E25"/>
@@ -2666,7 +2693,7 @@
       <c r="AA25" s="12"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="2:28" ht="18.95" customHeight="1">
+    <row r="26" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -2677,7 +2704,7 @@
       <c r="AA26" s="12"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="2:28" ht="18.95" customHeight="1">
+    <row r="27" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -2689,304 +2716,304 @@
       <c r="AA27" s="12"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="2:28" ht="18.95" customHeight="1">
+    <row r="28" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28"/>
       <c r="J28"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="2:28" ht="18.95" customHeight="1">
+    <row r="29" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29"/>
       <c r="J29"/>
       <c r="X29"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="2:28" ht="18.95" customHeight="1">
+    <row r="30" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30"/>
       <c r="J30"/>
       <c r="X30"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="2:28" ht="18.95" customHeight="1">
+    <row r="31" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31"/>
       <c r="J31"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="2:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="32" spans="2:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="33" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="34" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="35" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA35" s="12"/>
     </row>
-    <row r="36" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="36" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
       <c r="AA36" s="12"/>
     </row>
-    <row r="37" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="37" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z37" s="5"/>
       <c r="AA37" s="12"/>
     </row>
-    <row r="38" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="38" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
       <c r="AA38" s="12"/>
     </row>
-    <row r="39" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="39" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA39" s="12"/>
     </row>
-    <row r="40" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="40" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="41" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
       <c r="AA41" s="12"/>
     </row>
-    <row r="42" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="42" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z42" s="5"/>
       <c r="AA42" s="12"/>
     </row>
-    <row r="43" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="43" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="12"/>
     </row>
-    <row r="44" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="44" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="12"/>
     </row>
-    <row r="45" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="45" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA45" s="12"/>
     </row>
-    <row r="46" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="46" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA46" s="12"/>
     </row>
-    <row r="47" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="47" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
       <c r="AA47" s="12"/>
     </row>
-    <row r="48" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="48" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z48" s="5"/>
       <c r="AA48" s="12"/>
     </row>
-    <row r="49" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="49" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
       <c r="AA49" s="12"/>
     </row>
-    <row r="50" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="50" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
       <c r="AA50" s="12"/>
     </row>
-    <row r="51" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="51" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N51" s="14"/>
       <c r="AA51" s="12"/>
     </row>
-    <row r="52" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="52" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
       <c r="AA52" s="12"/>
     </row>
-    <row r="53" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="53" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z53" s="5"/>
       <c r="AA53" s="12"/>
     </row>
-    <row r="54" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="54" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA54" s="12"/>
     </row>
-    <row r="55" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="55" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
       <c r="AA55" s="12"/>
     </row>
-    <row r="56" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="56" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="U56" s="7"/>
       <c r="V56" s="7"/>
       <c r="Z56" s="12"/>
       <c r="AA56" s="12"/>
     </row>
-    <row r="57" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="57" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA57" s="12"/>
     </row>
-    <row r="58" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="58" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
       <c r="AA58" s="12"/>
     </row>
-    <row r="59" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="59" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V59" s="7"/>
       <c r="Z59" s="12"/>
       <c r="AA59" s="12"/>
     </row>
-    <row r="60" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="60" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N60" s="14"/>
       <c r="AA60" s="12"/>
     </row>
-    <row r="61" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="61" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
       <c r="AA61" s="12"/>
     </row>
-    <row r="62" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="62" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z62" s="5"/>
       <c r="AA62" s="12"/>
     </row>
-    <row r="63" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="63" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA63" s="12"/>
     </row>
-    <row r="64" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="64" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
       <c r="AA64" s="12"/>
     </row>
-    <row r="65" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="65" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y65" s="5"/>
       <c r="Z65" s="5"/>
       <c r="AA65" s="12"/>
     </row>
-    <row r="66" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="66" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
       <c r="AA66" s="12"/>
     </row>
-    <row r="67" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="67" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
       <c r="AA67" s="12"/>
     </row>
-    <row r="68" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="68" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA68" s="12"/>
     </row>
-    <row r="69" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="69" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z69" s="5"/>
       <c r="AA69" s="12"/>
     </row>
-    <row r="70" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="70" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
       <c r="AA70" s="12"/>
     </row>
-    <row r="71" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="71" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
       <c r="AA71" s="12"/>
     </row>
-    <row r="72" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="72" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA72" s="12"/>
     </row>
-    <row r="73" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="73" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z73" s="5"/>
       <c r="AA73" s="12"/>
     </row>
-    <row r="74" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="74" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y74" s="5"/>
       <c r="Z74" s="5"/>
       <c r="AA74" s="12"/>
     </row>
-    <row r="75" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="75" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z75" s="5"/>
       <c r="AA75" s="12"/>
     </row>
-    <row r="76" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="76" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
       <c r="AA76" s="12"/>
     </row>
-    <row r="77" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="77" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z77" s="5"/>
       <c r="AA77" s="12"/>
     </row>
-    <row r="78" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="78" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
     </row>
-    <row r="79" spans="7:27" ht="18.95" customHeight="1">
+    <row r="79" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="Z79" s="7"/>
       <c r="AA79" s="12"/>
     </row>
-    <row r="80" spans="7:27" ht="18.95" customHeight="1">
+    <row r="80" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="Z80" s="7"/>
       <c r="AA80" s="12"/>
     </row>
-    <row r="81" spans="7:27" ht="18.95" customHeight="1">
+    <row r="81" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="Z81" s="7"/>
       <c r="AA81" s="12"/>
     </row>
-    <row r="82" spans="7:27" ht="18.95" customHeight="1">
+    <row r="82" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="Z82" s="7"/>
       <c r="AA82" s="12"/>
     </row>
-    <row r="83" spans="7:27" ht="18.95" customHeight="1">
+    <row r="83" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="Z83" s="7"/>
       <c r="AA83" s="12"/>
     </row>
-    <row r="84" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="84" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z84" s="7"/>
       <c r="AA84" s="12"/>
     </row>
-    <row r="85" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="85" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z85" s="7"/>
       <c r="AA85" s="12"/>
     </row>
-    <row r="86" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="86" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z86" s="7"/>
       <c r="AA86" s="12"/>
     </row>
-    <row r="87" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="87" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z87" s="7"/>
       <c r="AA87" s="12"/>
     </row>
-    <row r="88" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="88" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z88" s="7"/>
       <c r="AA88" s="12"/>
     </row>
-    <row r="89" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="89" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y89" s="5"/>
       <c r="Z89" s="7"/>
       <c r="AA89" s="12"/>
     </row>
-    <row r="90" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="90" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y90" s="5"/>
       <c r="Z90" s="7"/>
       <c r="AA90" s="12"/>
     </row>
-    <row r="91" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="91" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y91" s="5"/>
       <c r="Z91" s="7"/>
       <c r="AA91" s="12"/>
     </row>
-    <row r="92" spans="7:27" ht="18.95" customHeight="1">
+    <row r="92" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y92" s="5"/>
       <c r="Z92" s="7"/>
       <c r="AA92" s="12"/>
     </row>
-    <row r="93" spans="7:27" ht="18.95" customHeight="1">
+    <row r="93" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cap for data consumer client
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B60532-6DF8-B245-B1B1-F6DBF6AA92D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B80D0A9-97BD-984A-8045-CE0EBF7C5DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="580" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="-20960" windowWidth="30040" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="155">
   <si>
     <t>Element</t>
   </si>
@@ -367,12 +367,6 @@
   </si>
   <si>
     <t>HL7 International - Patient Care Work Group</t>
-  </si>
-  <si>
-    <t>http://www.hl7.org/Special/committees/patientcare/index.cfm</t>
-  </si>
-  <si>
-    <t>0.2.0</t>
   </si>
   <si>
     <t xml:space="preserve">1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
@@ -390,18 +384,12 @@
 HRex Coverage Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
-  </si>
-  <si>
     <t>Required resource type to request and fetch clinical information from data source</t>
   </si>
   <si>
     <t>Subscription</t>
   </si>
   <si>
-    <t>Required resource type to fetch Clinical Information from data source</t>
-  </si>
-  <si>
     <t>Required resource type to subscribe to data source</t>
   </si>
   <si>
@@ -429,16 +417,6 @@
     <t>history-system</t>
   </si>
   <si>
-    <t>The  Da Vinci CDex Data Consumer  **SHALL**:
-1. Support at least one of the two FHIR transaction approaches for requesting information as defined in this Guide:
-     1. Direct Query
-     1. Task Based Approachs
-1. Support json source formats for all Da Vinci CDex interactions.
-1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
-The  Da Vinci CDex Data Consumer  **SHOULD**:
-1. Support xml source formats for all Da Vinci CDex interactions.</t>
-  </si>
-  <si>
     <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
   </si>
   <si>
@@ -451,107 +429,138 @@
     <t>data-consumer-client</t>
   </si>
   <si>
-    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Consumer (often a Payer) in *Client* mode when requesting clinical data from the Data Source (often an EHR) during a clinical data exchange.  This includes the following interactions:
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
+  </si>
+  <si>
+    <t>suppress_may_sps</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>json,xml</t>
+  </si>
+  <si>
+    <t>format_conf</t>
+  </si>
+  <si>
+    <t>SHALL,SHOULD</t>
+  </si>
+  <si>
+    <t>patchFormat</t>
+  </si>
+  <si>
+    <t>application/json-patch+json</t>
+  </si>
+  <si>
+    <t>patchFormat_conf</t>
+  </si>
+  <si>
+    <t>canonical</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>instantiates</t>
+  </si>
+  <si>
+    <t>US Core Client CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>include_conf</t>
+  </si>
+  <si>
+    <t>revinclude</t>
+  </si>
+  <si>
+    <t>revinclude_conf</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/profile-claim</t>
+  </si>
+  <si>
+    <t>PAS Claim</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition-profile-claim.html</t>
+  </si>
+  <si>
+    <t>conf_Claim</t>
+  </si>
+  <si>
+    <t>doc_Claim</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement-us-core-client.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/index.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
+  </si>
+  <si>
+    <t>http://www.hl7.org/Special/committees/patientcare</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Data Consumer Client CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/CapabilityStatement/data-consumer-client</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
+  </si>
+  <si>
+    <t>Resource type to carry information regarding reason for requesting information to support claim submission, medical necessity and other reasons for attachments between payers and providers, and 2) additional information to support prior authorization requests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Consumer (often a Payer) in *Client* mode when requesting clinical data from the Data Source (often an EHR) during a clinical data exchange.  This includes the following interactions:
 1. Requesting Clinical Data using a FHIR RESTful query
 1. POSTing a Task resource representing a request for clinical data
 1. POSTing a Subscription resource
-1. Polling a Task resource</t>
-  </si>
-  <si>
-    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
-  </si>
-  <si>
-    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
-    <t>suppress_may_sps</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>json,xml</t>
-  </si>
-  <si>
-    <t>format_conf</t>
-  </si>
-  <si>
-    <t>SHALL,SHOULD</t>
-  </si>
-  <si>
-    <t>patchFormat</t>
-  </si>
-  <si>
-    <t>application/json-patch+json</t>
-  </si>
-  <si>
-    <t>patchFormat_conf</t>
-  </si>
-  <si>
-    <t>canonical</t>
-  </si>
-  <si>
-    <t>imports</t>
-  </si>
-  <si>
-    <t>instantiates</t>
-  </si>
-  <si>
-    <t>US Core Client CapabilityStatement</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client</t>
-  </si>
-  <si>
-    <t>include</t>
-  </si>
-  <si>
-    <t>include_conf</t>
-  </si>
-  <si>
-    <t>revinclude</t>
-  </si>
-  <si>
-    <t>revinclude_conf</t>
-  </si>
-  <si>
-    <t>Claim</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/profile-claim</t>
-  </si>
-  <si>
-    <t>PAS Claim</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition-profile-claim.html</t>
-  </si>
-  <si>
-    <t>conf_Claim</t>
-  </si>
-  <si>
-    <t>doc_Claim</t>
-  </si>
-  <si>
-    <t>Resource type to carry information regarding reason for requesting  1) attachments to support claim submission, medical necessity and other reasons for attachments between payers and providers, and 2) additional information to support prior authorization requests.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement-us-core-client.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
+1. Polling a Task resource
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required resource type to fetch Clinical Information from data source. 
+</t>
+  </si>
+  <si>
+    <t>The  Da Vinci CDex Data Consumer  **SHALL**:
+1. Support at least one of these FHIR transaction approaches for exchanging clinical information as defined in this Guide:
+     1. Direct Query
+     1. Task Based Approach
+1. Follow the guidelines for [Generating and Verifying Signed Resources](signatures.html) *if signatures are required*.
+1. Support JSON source formats for all Da Vinci CDex interactions.
+1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
+The  Da Vinci CDex Data Consumer **SHOULD**:
+1. Support xml source formats for all Da Vinci CDex interactions.</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1052,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1070,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1070,7 +1079,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1110,12 +1119,12 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
@@ -1134,7 +1143,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2353,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2376,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2384,7 +2393,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2400,7 +2409,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2416,7 +2425,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2424,39 +2433,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2466,31 +2475,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A085B-7918-1B43-BDD7-DE64008365F6}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>88</v>
@@ -2505,15 +2514,32 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2542,7 +2568,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>88</v>
@@ -2553,13 +2579,13 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2567,13 +2593,13 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -2589,7 +2615,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2620,25 +2646,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
@@ -2651,36 +2677,36 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2720,7 +2746,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2804,43 +2830,43 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -2848,18 +2874,18 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="22:25" ht="18" x14ac:dyDescent="0.2">
@@ -2881,7 +2907,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2931,7 +2957,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2948,10 +2974,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
@@ -2960,16 +2986,16 @@
         <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3154,7 +3180,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3177,7 +3203,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -3187,7 +3213,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
@@ -3195,7 +3221,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>25</v>
@@ -3203,7 +3229,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
update capstatements source files
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B80D0A9-97BD-984A-8045-CE0EBF7C5DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B968DAA-E069-6640-A257-04B3F15E6108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-20960" windowWidth="30040" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12160" yWindow="-20280" windowWidth="30040" windowHeight="20920" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -25,10 +25,13 @@
     <sheet name="sps" sheetId="7" r:id="rId10"/>
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId12"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$B$1:$B$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$92</definedName>
-    <definedName name="profile" localSheetId="4">profiles!$A$6</definedName>
+    <definedName name="profile" localSheetId="4">[1]profiles!$A$2</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -750,6 +753,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="config"/>
+      <sheetName val="meta"/>
+      <sheetName val="capstatements"/>
+      <sheetName val="igs"/>
+      <sheetName val="profiles"/>
+      <sheetName val="resources"/>
+      <sheetName val="ops"/>
+      <sheetName val="interactions"/>
+      <sheetName val="rest_interactions"/>
+      <sheetName val="sps"/>
+      <sheetName val="sp_combos"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2362,7 +2404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2478,7 +2520,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2614,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2710,9 +2752,6 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="1"/>
-    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G7" s="1"/>
     </row>
@@ -2746,7 +2785,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update to HREX 1.0.0
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8451E1-7ED2-804C-B533-56D5A73B8440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4451CFD-3C34-7943-9558-3B511788C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18920" yWindow="-21140" windowWidth="30040" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18920" yWindow="-21140" windowWidth="30040" windowHeight="20920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -435,15 +435,9 @@
     <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
   </si>
   <si>
-    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
-  </si>
-  <si>
     <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
     <t>suppress_may_sps</t>
   </si>
   <si>
@@ -517,9 +511,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
   </si>
   <si>
     <t>http://www.hl7.org/Special/committees/patientcare</t>
@@ -564,12 +555,21 @@
 1. POSTing a Subscription resource
 1. Polling a Task resource</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|1.0.0</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 1.0.0 - STU R1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/STU1/index.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +659,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -701,11 +709,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -736,9 +745,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1111,7 +1122,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1120,7 +1131,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1160,12 +1171,12 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
@@ -2403,7 +2414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2434,7 +2445,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2450,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2466,7 +2477,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,31 +2490,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -2531,16 +2542,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>88</v>
@@ -2555,13 +2566,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -2572,13 +2583,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -2593,13 +2604,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.33203125" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" style="1" customWidth="1"/>
   </cols>
@@ -2609,7 +2620,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>88</v>
@@ -2626,7 +2637,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2634,19 +2645,23 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CB84C727-891D-FD46-B678-86467D7F6F7B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A5FB987A-CAC7-F54A-9172-33E3F467A04C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2702,7 +2717,7 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>99</v>
@@ -2735,19 +2750,19 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2868,27 +2883,27 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="2"/>
@@ -2912,7 +2927,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
@@ -3012,10 +3027,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
update to pub ver of hrex
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8451E1-7ED2-804C-B533-56D5A73B8440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4451CFD-3C34-7943-9558-3B511788C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18920" yWindow="-21140" windowWidth="30040" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18920" yWindow="-21140" windowWidth="30040" windowHeight="20920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -435,15 +435,9 @@
     <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
   </si>
   <si>
-    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
-  </si>
-  <si>
     <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
     <t>suppress_may_sps</t>
   </si>
   <si>
@@ -517,9 +511,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
   </si>
   <si>
     <t>http://www.hl7.org/Special/committees/patientcare</t>
@@ -564,12 +555,21 @@
 1. POSTing a Subscription resource
 1. Polling a Task resource</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|1.0.0</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 1.0.0 - STU R1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/STU1/index.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +659,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -701,11 +709,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -736,9 +745,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1111,7 +1122,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1120,7 +1131,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1160,12 +1171,12 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
@@ -2403,7 +2414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2434,7 +2445,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2450,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2466,7 +2477,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,31 +2490,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -2531,16 +2542,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>88</v>
@@ -2555,13 +2566,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -2572,13 +2583,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -2593,13 +2604,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.33203125" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" style="1" customWidth="1"/>
   </cols>
@@ -2609,7 +2620,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>88</v>
@@ -2626,7 +2637,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2634,19 +2645,23 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CB84C727-891D-FD46-B678-86467D7F6F7B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A5FB987A-CAC7-F54A-9172-33E3F467A04C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2702,7 +2717,7 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>99</v>
@@ -2735,19 +2750,19 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2868,27 +2883,27 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="2"/>
@@ -2912,7 +2927,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
@@ -3012,10 +3027,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Pre-Apply - Clarify support for XML with signatures FHIR-37264
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4451CFD-3C34-7943-9558-3B511788C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CA16C8-08B1-0F4D-A6DA-F0C477D8C2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18920" yWindow="-21140" windowWidth="30040" windowHeight="20920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1760" windowWidth="30040" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -435,9 +435,6 @@
     <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
   </si>
   <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
-  </si>
-  <si>
     <t>suppress_may_sps</t>
   </si>
   <si>
@@ -448,9 +445,6 @@
   </si>
   <si>
     <t>format_conf</t>
-  </si>
-  <si>
-    <t>SHALL,SHOULD</t>
   </si>
   <si>
     <t>patchFormat</t>
@@ -533,6 +527,31 @@
   <si>
     <t xml:space="preserve">Required resource type to fetch Clinical Information from data source. 
 </t>
+  </si>
+  <si>
+    <t>http://build.fhir.org/ig/HL7/davinci-ecdx/package.tgz</t>
+  </si>
+  <si>
+    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Consumer (often a Payer) in *Client* mode when requesting clinical data from the Data Source (often an EHR) during a clinical data exchange.  This includes the following interactions:
+1. Requesting Clinical Data using a FHIR RESTful query
+1. POSTing a Task resource representing a request for clinical data
+1. POSTing a Subscription resource
+1. Polling a Task resource</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|1.0.0</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 1.0.0 - STU R1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/STU1/index.html</t>
+  </si>
+  <si>
+    <t>SHALL,MAY</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-ecdx/input/</t>
   </si>
   <si>
     <t>The  Da Vinci CDex Data Consumer  **SHALL**:
@@ -542,27 +561,9 @@
 1. Follow the guidelines for [Generating and Verifying Signed Resources](signatures.html) *if signatures are required*.
 1. Support JSON source formats for all Da Vinci CDex interactions.
 1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
-The  Da Vinci CDex Data Consumer **SHOULD**:
-1. Support xml source formats for all Da Vinci CDex interactions.</t>
-  </si>
-  <si>
-    <t>http://build.fhir.org/ig/HL7/davinci-ecdx/package.tgz</t>
-  </si>
-  <si>
-    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Consumer (often a Payer) in *Client* mode when requesting clinical data from the Data Source (often an EHR) during a clinical data exchange.  This includes the following interactions:
-1. Requesting Clinical Data using a FHIR RESTful query
-1. POSTing a Task resource representing a request for clinical data
-1. POSTing a Subscription resource
-1. Polling a Task resource</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|1.0.0</t>
-  </si>
-  <si>
-    <t>Da Vinci Health Record Exchange (HRex) 1.0.0 - STU R1</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/STU1/index.html</t>
+The  Da Vinci CDex Data Consumer **MAY**:
+1. Support XML source formats for all Da Vinci CDex interactions.
+   &gt; Implementers that choose to support XML need to be aware that JSON Web Signatures can only be created and validated in the original native JSON.  Transforms to and from XML will invalidate signatures.</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1105,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1123,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1131,7 +1132,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1171,12 +1172,12 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
@@ -2414,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2445,7 +2446,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2461,7 +2462,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2477,7 +2478,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2490,31 +2491,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -2542,16 +2543,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>88</v>
@@ -2566,13 +2567,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -2583,13 +2584,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -2604,7 +2605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2620,7 +2621,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>88</v>
@@ -2637,7 +2638,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2645,13 +2646,13 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -2717,7 +2718,7 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>99</v>
@@ -2750,19 +2751,19 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2883,27 +2884,27 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="2"/>
@@ -2927,7 +2928,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
@@ -3027,10 +3028,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Update to US Core 6.1, fix QA issues arrising from the updates and new publisher version
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9AEE05-DCA2-A740-AF77-ABF3FC93217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294BB416-BC58-054A-A9D6-0BD131F2968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="500" windowWidth="34120" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34040" yWindow="500" windowWidth="33900" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="191">
   <si>
     <t>Element</t>
   </si>
@@ -441,12 +441,6 @@
     <t>instantiates</t>
   </si>
   <si>
-    <t>US Core Client CapabilityStatement</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
@@ -459,19 +453,7 @@
     <t>revinclude_conf</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement-us-core-client.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
     <t>http://www.hl7.org/Special/committees/patientcare</t>
-  </si>
-  <si>
-    <t>Data Consumer Client CapabilityStatement</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-cdex/CapabilityStatement/data-consumer-client</t>
   </si>
   <si>
     <t>http://build.fhir.org/ig/HL7/davinci-ecdx/package.tgz</t>
@@ -582,9 +564,6 @@
    - *CDex Task Attachment Request Profile*
    - *CDex Patient Demographic Profile*
    - *CDex PractitionerRequest Profile*</t>
-  </si>
-  <si>
-    <t>2.0.0</t>
   </si>
   <si>
     <t>The  Da Vinci CDex Data Consumer Client  **SHALL**:
@@ -614,28 +593,7 @@
     <t>QuestionnaireResponse</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-dtr/StructureDefinition/dtr-sdc-questionnaire</t>
-  </si>
-  <si>
-    <t>DTR SDC Questionnaire</t>
-  </si>
-  <si>
     <t>Questionnaire</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-dtr/StructureDefinition/dtr-sdc-questionnaire-adapt</t>
-  </si>
-  <si>
-    <t>DTR SDC Questionnaire for adaptive form</t>
-  </si>
-  <si>
-    <t>Documentation Templates and Rules 1.1.0-ballot</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-dtr/ImplementationGuide/hl7.fhir.us.davinci-dtr|1.1.0-ballot</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-dtr/2022May/index.html</t>
   </si>
   <si>
     <t>Required resource type to  when requesting data or attachments using Questionnaire</t>
@@ -685,14 +643,81 @@
    - Requesting Attachments Using Attachments Codes
    - Requesting Attachments Using Questionnaires</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client|3.1.1</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/core/STU3.1.1/CapabilityStatement-us-core-client.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client|6.1.0</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/core/STU6.1.0/CapabilityStatement-us-core-client.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/STU3.1.1/index.html</t>
+  </si>
+  <si>
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 6.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core|6.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/STU6.1.0/index.html</t>
+  </si>
+  <si>
+    <t>Documentation Templates and Rules 2.0.1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-dtr/ImplementationGuide/hl7.fhir.us.davinci-dtr|2.0.1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-dtr/STU2.0.1/index.html</t>
+  </si>
+  <si>
+    <t>US Core Version 3.1.1 Client CapabilityStatement</t>
+  </si>
+  <si>
+    <t>US Core Version 6.1.0 Client CapabilityStatement</t>
+  </si>
+  <si>
+    <t>2.1.0-preview</t>
+  </si>
+  <si>
+    <t>DTR Standard Questionnaire</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/davinci-dtr/STU2/StructureDefinition-dtr-std-questionnaire.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-dtr/StructureDefinition/dtr-std-questionnaire</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-dtr/StructureDefinition/dtr-questionnaire-adapt</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/davinci-dtr/STU2/StructureDefinition-dtr-questionnaire-adapt.html</t>
+  </si>
+  <si>
+    <t>DTR Questionnaire for adaptive form</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -798,20 +823,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -878,12 +889,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -891,42 +901,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -943,8 +950,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="config"/>
       <sheetName val="meta"/>
@@ -982,9 +992,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1022,7 +1032,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1128,7 +1138,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1270,7 +1280,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1299,7 +1309,7 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1307,7 +1317,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1347,7 +1357,7 @@
         <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2287,7 +2297,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2317,7 +2327,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2333,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2349,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2357,7 +2367,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2373,7 +2383,7 @@
         <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2401,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A085B-7918-1B43-BDD7-DE64008365F6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2432,38 +2442,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>129</v>
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" t="s">
+        <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>125</v>
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2473,10 +2483,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2507,46 +2517,55 @@
         <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>133</v>
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>176</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{CB84C727-891D-FD46-B678-86467D7F6F7B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{A5FB987A-CAC7-F54A-9172-33E3F467A04C}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{ED365816-6A83-4F46-8D71-00D2C595E013}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2555,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2569,158 +2588,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="C2" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="A3" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>142</v>
+      <c r="E5" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>152</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>169</v>
+        <v>159</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>171</v>
+        <v>187</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>172</v>
+        <v>186</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>174</v>
+        <v>188</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>172</v>
+        <v>189</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2733,11 +2752,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:C9"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2821,16 +2840,16 @@
         <v>73</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="234" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2841,7 +2860,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="48" x14ac:dyDescent="0.2">
@@ -2852,7 +2871,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
@@ -2863,66 +2882,66 @@
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>179</v>
+      <c r="C8" s="23" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C22" s="25"/>
+      <c r="C22"/>
     </row>
     <row r="23" spans="3:25" ht="18" x14ac:dyDescent="0.2">
       <c r="V23" s="6"/>
@@ -3030,34 +3049,34 @@
         <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="M1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="N1" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="O1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="P1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="Q1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
**Pre-Applied:** (Enhancement) update to support topic based subscriptions [FHIR-45628]
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294BB416-BC58-054A-A9D6-0BD131F2968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AD3229-EEC5-614F-8945-D9A70D4A14F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34040" yWindow="500" windowWidth="33900" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34040" yWindow="500" windowWidth="33900" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="194">
   <si>
     <t>Element</t>
   </si>
@@ -702,6 +702,15 @@
   </si>
   <si>
     <t>DTR Questionnaire for adaptive form</t>
+  </si>
+  <si>
+    <t>Subscriptions R5 Backport (FHIR IG) Release 1.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/uv/subscriptions-backport/ImplementationGuide/hl7.fhir.uv.subscriptions-backport|1.1.0</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/</t>
   </si>
 </sst>
 </file>
@@ -2483,10 +2492,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2565,6 +2574,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2574,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Pre-Apply: Support both US-Core 3.1.1 and 6.1.0 and 7.0.0 FHIR-47303
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-client.xlsx
+++ b/input/resources-spreadsheet/data-consumer-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AD3229-EEC5-614F-8945-D9A70D4A14F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF459946-D53A-A346-A7B5-00D819EB635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34040" yWindow="500" windowWidth="33900" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="71380" yWindow="500" windowWidth="33900" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="200">
   <si>
     <t>Element</t>
   </si>
@@ -711,6 +711,24 @@
   </si>
   <si>
     <t>https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/</t>
+  </si>
+  <si>
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 7.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core|7.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/STU7.0.0/index.html</t>
+  </si>
+  <si>
+    <t>US Core Version 7.0.0 Client CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-client|7.0.0</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/core/STU7.0.0/CapabilityStatement-us-core-client.html</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1003,7 @@
       <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
-            <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+            <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference|3.1.1</v>
           </cell>
         </row>
       </sheetData>
@@ -2418,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A085B-7918-1B43-BDD7-DE64008365F6}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2485,6 +2503,23 @@
         <v>52</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2492,10 +2527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2548,43 +2583,57 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>126</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>127</v>
       </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>180</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>181</v>
       </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>191</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>192</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>193</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2597,7 +2646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>